<commit_message>
creta vendor contact done
</commit_message>
<xml_diff>
--- a/catatan/new.xlsx
+++ b/catatan/new.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="438">
   <si>
     <t>Master</t>
   </si>
@@ -1092,9 +1092,6 @@
     <t>PT. Segar Makmur - Gudang Sidoarjo</t>
   </si>
   <si>
-    <t>PT. Segar Makmu - HO</t>
-  </si>
-  <si>
     <t>PT. Segar Makmur - Gudang Mojokerto</t>
   </si>
   <si>
@@ -1240,10 +1237,193 @@
   </si>
   <si>
     <t>BOX                            ˅</t>
+  </si>
+  <si>
+    <t>˅</t>
+  </si>
+  <si>
+    <t>Master Customer, Vendor, Ekspedisi</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Surabaya      </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jawa Timur    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Retail A1             </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sidoarjo                </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
   </si>
   <si>
     <r>
       <t xml:space="preserve">Jawa Timur          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">SBY KT-SDA KT    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mojokerto           </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Non Franco          </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Surabaya     </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jawa Timur </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>˅</t>
+    </r>
+  </si>
+  <si>
+    <t>Kode</t>
+  </si>
+  <si>
+    <t>Tempat Bongkar</t>
+  </si>
+  <si>
+    <t>Tempat Muat</t>
+  </si>
+  <si>
+    <t>Tarif</t>
+  </si>
+  <si>
+    <t>Jarak</t>
+  </si>
+  <si>
+    <t>Depo Jember</t>
+  </si>
+  <si>
+    <t>200 Km</t>
+  </si>
+  <si>
+    <t>internal depo</t>
+  </si>
+  <si>
+    <t>AQPDN-DPJBR</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Jember                                              </t>
     </r>
     <r>
       <rPr>
@@ -1259,7 +1439,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">SBY KT-SDA KT    </t>
+      <t xml:space="preserve">Pandaaan, Pasuruan           </t>
     </r>
     <r>
       <rPr>
@@ -1274,145 +1454,59 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Sidoarjo                </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mojokerto           </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Non Franco          </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Jawa Timur    </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Retail A1             </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Surabaya      </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <t>˅</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Surabaya     </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Jawa Timur </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>˅</t>
-    </r>
-  </si>
-  <si>
-    <t>Master Customer, Vendor, Ekspedisi</t>
+    <t>Nama Program</t>
+  </si>
+  <si>
+    <t>Nama Produk</t>
+  </si>
+  <si>
+    <t>Pot %</t>
+  </si>
+  <si>
+    <t>Pot Rp</t>
+  </si>
+  <si>
+    <t>Add Line</t>
+  </si>
+  <si>
+    <t>Aqua Galon</t>
+  </si>
+  <si>
+    <t>Grup Customer</t>
+  </si>
+  <si>
+    <t>Retail A1</t>
+  </si>
+  <si>
+    <t>Min QTY</t>
+  </si>
+  <si>
+    <t>Detail Program</t>
+  </si>
+  <si>
+    <t>Periode Program</t>
+  </si>
+  <si>
+    <t>11/1/2021          s/d</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Customer </t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>GLN-RTLA1-NOV21</t>
+  </si>
+  <si>
+    <t>Program Galon Retail A1 Potongan 2 %</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1436,8 +1530,21 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="14"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1445,7 +1552,6 @@
     <font>
       <u/>
       <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1508,18 +1614,18 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0"/>
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="24">
     <border>
       <left/>
       <right/>
@@ -1696,12 +1802,92 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="160">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1806,24 +1992,17 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1866,11 +2045,26 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1881,83 +2075,172 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="12" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="4" fillId="9" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4593,7 +4876,7 @@
   <dimension ref="A1:P30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4613,7 +4896,7 @@
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="122" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
@@ -4664,7 +4947,7 @@
       <c r="M3" s="20"/>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="B4" s="122" t="s">
         <v>4</v>
       </c>
       <c r="C4" t="s">
@@ -4682,7 +4965,7 @@
       <c r="M4" s="20"/>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+      <c r="B5" s="122" t="s">
         <v>5</v>
       </c>
       <c r="C5" t="s">
@@ -4707,7 +4990,7 @@
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="B6" s="122" t="s">
         <v>6</v>
       </c>
       <c r="C6" t="s">
@@ -4732,7 +5015,7 @@
         <v>179</v>
       </c>
       <c r="E7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="19"/>
@@ -4744,7 +5027,7 @@
         <v>8</v>
       </c>
       <c r="C8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="J8" s="25" t="s">
         <v>115</v>
@@ -4756,7 +5039,7 @@
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="B9" s="122" t="s">
         <v>28</v>
       </c>
       <c r="C9" t="s">
@@ -4895,629 +5178,1575 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="A1:V37"/>
+  <dimension ref="A1:X56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" topLeftCell="E37" workbookViewId="0">
+      <selection activeCell="P61" sqref="P61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" customWidth="1"/>
     <col min="3" max="4" width="12.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" customWidth="1"/>
+    <col min="5" max="5" width="17.5703125" customWidth="1"/>
     <col min="6" max="6" width="15" customWidth="1"/>
     <col min="7" max="7" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.5703125" customWidth="1"/>
     <col min="9" max="9" width="3.140625" customWidth="1"/>
-    <col min="11" max="11" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" customWidth="1"/>
     <col min="12" max="12" width="16.42578125" customWidth="1"/>
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
     <col min="14" max="14" width="10.5703125" customWidth="1"/>
     <col min="15" max="15" width="14.42578125" customWidth="1"/>
+    <col min="16" max="16" width="10" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.5703125" customWidth="1"/>
     <col min="18" max="18" width="23.42578125" customWidth="1"/>
     <col min="19" max="19" width="12.140625" customWidth="1"/>
     <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="11.5703125" customWidth="1"/>
     <col min="22" max="22" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A1" s="78" t="s">
+        <v>400</v>
+      </c>
+      <c r="B1" s="79"/>
+      <c r="C1" s="79"/>
+      <c r="D1" s="79"/>
+      <c r="E1" s="79"/>
+      <c r="F1" s="79"/>
+      <c r="G1" s="79"/>
+      <c r="H1" s="79"/>
+      <c r="I1" s="79"/>
+      <c r="J1" s="79"/>
+      <c r="K1" s="79"/>
+      <c r="L1" s="79"/>
+      <c r="M1" s="79"/>
+      <c r="N1" s="79"/>
+      <c r="O1" s="79"/>
+      <c r="P1" s="79"/>
+      <c r="Q1" s="79"/>
+      <c r="R1" s="79"/>
+      <c r="S1" s="79"/>
+      <c r="T1" s="79"/>
+      <c r="U1" s="79"/>
+      <c r="V1" s="79"/>
+      <c r="W1" s="80"/>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A2" s="81"/>
+      <c r="B2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
+      <c r="N2" s="82"/>
+      <c r="O2" s="82"/>
+      <c r="P2" s="82"/>
+      <c r="Q2" s="82"/>
+      <c r="R2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="83"/>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A3" s="81"/>
+      <c r="B3" s="82" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="84" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="82"/>
+      <c r="E3" s="84" t="s">
+        <v>341</v>
+      </c>
+      <c r="F3" s="82"/>
+      <c r="G3" s="84" t="s">
+        <v>79</v>
+      </c>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
+      <c r="O3" s="82"/>
+      <c r="P3" s="82"/>
+      <c r="Q3" s="82"/>
+      <c r="R3" s="82"/>
+      <c r="S3" s="82"/>
+      <c r="T3" s="82"/>
+      <c r="U3" s="82"/>
+      <c r="V3" s="82"/>
+      <c r="W3" s="83"/>
+    </row>
+    <row r="4" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="81"/>
+      <c r="B4" s="85" t="s">
+        <v>379</v>
+      </c>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="87"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
+      <c r="N4" s="82"/>
+      <c r="O4" s="82"/>
+      <c r="P4" s="82"/>
+      <c r="Q4" s="82"/>
+      <c r="R4" s="82"/>
+      <c r="S4" s="82"/>
+      <c r="T4" s="82"/>
+      <c r="U4" s="82"/>
+      <c r="V4" s="82"/>
+      <c r="W4" s="83"/>
+    </row>
+    <row r="5" spans="1:23" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="81"/>
+      <c r="B5" s="88" t="s">
+        <v>380</v>
+      </c>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="89"/>
+      <c r="F5" s="90"/>
+      <c r="G5" s="82"/>
+      <c r="H5" s="82"/>
+      <c r="I5" s="82"/>
+      <c r="J5" s="82"/>
+      <c r="K5" s="82"/>
+      <c r="L5" s="82"/>
+      <c r="M5" s="82"/>
+      <c r="N5" s="82"/>
+      <c r="O5" s="82"/>
+      <c r="P5" s="82"/>
+      <c r="Q5" s="82"/>
+      <c r="R5" s="82"/>
+      <c r="S5" s="82"/>
+      <c r="T5" s="82"/>
+      <c r="U5" s="82"/>
+      <c r="V5" s="82"/>
+      <c r="W5" s="83"/>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A6" s="81"/>
+      <c r="B6" s="82"/>
+      <c r="C6" s="82"/>
+      <c r="D6" s="82"/>
+      <c r="E6" s="82"/>
+      <c r="F6" s="82"/>
+      <c r="G6" s="82"/>
+      <c r="H6" s="82"/>
+      <c r="I6" s="82"/>
+      <c r="J6" s="82"/>
+      <c r="K6" s="82"/>
+      <c r="L6" s="82"/>
+      <c r="M6" s="82"/>
+      <c r="N6" s="82"/>
+      <c r="O6" s="82"/>
+      <c r="P6" s="82"/>
+      <c r="Q6" s="82"/>
+      <c r="R6" s="82"/>
+      <c r="S6" s="82"/>
+      <c r="T6" s="82"/>
+      <c r="U6" s="82"/>
+      <c r="V6" s="82"/>
+      <c r="W6" s="83"/>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A7" s="81"/>
+      <c r="B7" s="82" t="s">
+        <v>138</v>
+      </c>
+      <c r="C7" s="82" t="s">
+        <v>378</v>
+      </c>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82" t="s">
+        <v>137</v>
+      </c>
+      <c r="H7" s="82" t="s">
+        <v>381</v>
+      </c>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
+      <c r="O7" s="82"/>
+      <c r="P7" s="82"/>
+      <c r="Q7" s="82"/>
+      <c r="R7" s="82"/>
+      <c r="S7" s="82"/>
+      <c r="T7" s="82"/>
+      <c r="U7" s="82"/>
+      <c r="V7" s="82"/>
+      <c r="W7" s="83"/>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A8" s="81"/>
+      <c r="B8" s="82"/>
+      <c r="C8" s="82"/>
+      <c r="D8" s="82"/>
+      <c r="E8" s="82"/>
+      <c r="F8" s="82"/>
+      <c r="G8" s="82" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="91" t="s">
+        <v>382</v>
+      </c>
+      <c r="I8" s="82"/>
+      <c r="J8" s="82"/>
+      <c r="K8" s="82"/>
+      <c r="L8" s="82"/>
+      <c r="M8" s="82"/>
+      <c r="N8" s="82"/>
+      <c r="O8" s="82"/>
+      <c r="P8" s="82"/>
+      <c r="Q8" s="82"/>
+      <c r="R8" s="82"/>
+      <c r="S8" s="82"/>
+      <c r="T8" s="82"/>
+      <c r="U8" s="82"/>
+      <c r="V8" s="82"/>
+      <c r="W8" s="83"/>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A9" s="81"/>
+      <c r="B9" s="82"/>
+      <c r="C9" s="82" t="s">
+        <v>342</v>
+      </c>
+      <c r="D9" s="82" t="s">
+        <v>401</v>
+      </c>
+      <c r="E9" s="82" t="s">
+        <v>343</v>
+      </c>
+      <c r="F9" s="82" t="s">
+        <v>402</v>
+      </c>
+      <c r="G9" s="82" t="s">
+        <v>344</v>
+      </c>
+      <c r="H9" s="82" t="s">
+        <v>403</v>
+      </c>
+      <c r="I9" s="82"/>
+      <c r="J9" s="82"/>
+      <c r="K9" s="82"/>
+      <c r="L9" s="82"/>
+      <c r="M9" s="82"/>
+      <c r="N9" s="82"/>
+      <c r="O9" s="82"/>
+      <c r="P9" s="82"/>
+      <c r="Q9" s="82"/>
+      <c r="R9" s="82"/>
+      <c r="S9" s="82"/>
+      <c r="T9" s="82"/>
+      <c r="U9" s="82"/>
+      <c r="V9" s="82"/>
+      <c r="W9" s="83"/>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A10" s="81"/>
+      <c r="B10" s="82" t="s">
+        <v>140</v>
+      </c>
+      <c r="C10" s="82" t="s">
+        <v>383</v>
+      </c>
+      <c r="D10" s="82"/>
+      <c r="E10" s="82"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
+      <c r="N10" s="82"/>
+      <c r="O10" s="82"/>
+      <c r="P10" s="82"/>
+      <c r="Q10" s="82"/>
+      <c r="R10" s="82"/>
+      <c r="S10" s="82"/>
+      <c r="T10" s="82"/>
+      <c r="U10" s="82"/>
+      <c r="V10" s="82"/>
+      <c r="W10" s="83"/>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A11" s="81"/>
+      <c r="B11" s="82"/>
+      <c r="C11" s="82"/>
+      <c r="D11" s="82"/>
+      <c r="E11" s="82"/>
+      <c r="F11" s="82"/>
+      <c r="G11" s="82"/>
+      <c r="H11" s="82"/>
+      <c r="I11" s="82"/>
+      <c r="J11" s="82"/>
+      <c r="K11" s="82"/>
+      <c r="L11" s="82"/>
+      <c r="M11" s="82"/>
+      <c r="N11" s="82"/>
+      <c r="O11" s="82"/>
+      <c r="P11" s="82"/>
+      <c r="Q11" s="82"/>
+      <c r="R11" s="82"/>
+      <c r="S11" s="82"/>
+      <c r="T11" s="82"/>
+      <c r="U11" s="82"/>
+      <c r="V11" s="82"/>
+      <c r="W11" s="83"/>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A12" s="81"/>
+      <c r="B12" s="82"/>
+      <c r="C12" s="82"/>
+      <c r="D12" s="82"/>
+      <c r="E12" s="82"/>
+      <c r="F12" s="82"/>
+      <c r="G12" s="82"/>
+      <c r="H12" s="82"/>
+      <c r="I12" s="82"/>
+      <c r="J12" s="82"/>
+      <c r="K12" s="82"/>
+      <c r="L12" s="82"/>
+      <c r="M12" s="82"/>
+      <c r="N12" s="82"/>
+      <c r="O12" s="82"/>
+      <c r="P12" s="82"/>
+      <c r="Q12" s="82"/>
+      <c r="R12" s="82"/>
+      <c r="S12" s="82"/>
+      <c r="T12" s="82"/>
+      <c r="U12" s="82"/>
+      <c r="V12" s="82"/>
+      <c r="W12" s="83"/>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A13" s="81"/>
+      <c r="B13" s="152" t="s">
+        <v>142</v>
+      </c>
+      <c r="C13" s="92" t="s">
+        <v>368</v>
+      </c>
+      <c r="D13" s="93"/>
+      <c r="E13" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="F13" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="G13" s="82"/>
+      <c r="H13" s="82"/>
+      <c r="I13" s="82"/>
+      <c r="J13" s="82"/>
+      <c r="K13" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="L13" s="75" t="s">
+        <v>368</v>
+      </c>
+      <c r="M13" s="76"/>
+      <c r="N13" s="94" t="s">
+        <v>371</v>
+      </c>
+      <c r="O13" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="P13" s="82"/>
+      <c r="Q13" s="82"/>
+      <c r="R13" s="95" t="s">
+        <v>142</v>
+      </c>
+      <c r="S13" s="96" t="s">
+        <v>368</v>
+      </c>
+      <c r="T13" s="97"/>
+      <c r="U13" s="77" t="s">
+        <v>371</v>
+      </c>
+      <c r="V13" s="94" t="s">
+        <v>141</v>
+      </c>
+      <c r="W13" s="83"/>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A14" s="81"/>
+      <c r="B14" s="82"/>
+      <c r="C14" s="82"/>
+      <c r="D14" s="82"/>
+      <c r="E14" s="82"/>
+      <c r="F14" s="82"/>
+      <c r="G14" s="82"/>
+      <c r="H14" s="82"/>
+      <c r="I14" s="82"/>
+      <c r="J14" s="82"/>
+      <c r="K14" s="94" t="s">
+        <v>370</v>
+      </c>
+      <c r="L14" s="82"/>
+      <c r="M14" s="82"/>
+      <c r="N14" s="82"/>
+      <c r="O14" s="82"/>
+      <c r="P14" s="82"/>
+      <c r="Q14" s="82"/>
+      <c r="R14" s="82"/>
+      <c r="S14" s="82"/>
+      <c r="T14" s="82"/>
+      <c r="U14" s="82"/>
+      <c r="V14" s="82"/>
+      <c r="W14" s="83"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A15" s="81"/>
+      <c r="B15" s="98"/>
+      <c r="C15" s="99" t="s">
+        <v>354</v>
+      </c>
+      <c r="D15" s="99"/>
+      <c r="E15" s="99"/>
+      <c r="F15" s="100"/>
+      <c r="G15" s="82"/>
+      <c r="H15" s="82"/>
+      <c r="I15" s="82"/>
+      <c r="J15" s="82"/>
+      <c r="K15" s="82"/>
+      <c r="L15" s="82"/>
+      <c r="M15" s="82"/>
+      <c r="N15" s="82"/>
+      <c r="O15" s="82"/>
+      <c r="P15" s="82"/>
+      <c r="Q15" s="82"/>
+      <c r="R15" s="101" t="s">
+        <v>372</v>
+      </c>
+      <c r="S15" s="82"/>
+      <c r="T15" s="82"/>
+      <c r="U15" s="82"/>
+      <c r="V15" s="82"/>
+      <c r="W15" s="83"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A16" s="81"/>
+      <c r="B16" s="102"/>
+      <c r="C16" s="82" t="s">
+        <v>351</v>
+      </c>
+      <c r="D16" s="82"/>
+      <c r="E16" s="82"/>
+      <c r="F16" s="103"/>
+      <c r="G16" s="82"/>
+      <c r="H16" s="82"/>
+      <c r="I16" s="82"/>
+      <c r="J16" s="82"/>
+      <c r="K16" s="98" t="s">
+        <v>347</v>
+      </c>
+      <c r="L16" s="99" t="s">
+        <v>349</v>
+      </c>
+      <c r="M16" s="99"/>
+      <c r="N16" s="99"/>
+      <c r="O16" s="100"/>
+      <c r="P16" s="82"/>
+      <c r="Q16" s="82"/>
+      <c r="R16" s="104" t="s">
+        <v>80</v>
+      </c>
+      <c r="S16" s="104" t="s">
+        <v>72</v>
+      </c>
+      <c r="T16" s="104" t="s">
+        <v>374</v>
+      </c>
+      <c r="U16" s="104" t="s">
+        <v>373</v>
+      </c>
+      <c r="V16" s="104" t="s">
+        <v>141</v>
+      </c>
+      <c r="W16" s="83"/>
+    </row>
+    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A17" s="81"/>
+      <c r="B17" s="105"/>
+      <c r="C17" s="106" t="s">
+        <v>352</v>
+      </c>
+      <c r="D17" s="82"/>
+      <c r="E17" s="82"/>
+      <c r="F17" s="103"/>
+      <c r="G17" s="82"/>
+      <c r="H17" s="82"/>
+      <c r="I17" s="82"/>
+      <c r="J17" s="82"/>
+      <c r="K17" s="107"/>
+      <c r="L17" s="82" t="s">
+        <v>358</v>
+      </c>
+      <c r="M17" s="82"/>
+      <c r="N17" s="82"/>
+      <c r="O17" s="103"/>
+      <c r="P17" s="82"/>
+      <c r="Q17" s="82"/>
+      <c r="R17" s="95" t="s">
+        <v>395</v>
+      </c>
+      <c r="S17" s="95" t="s">
+        <v>397</v>
+      </c>
+      <c r="T17" s="95" t="s">
+        <v>398</v>
+      </c>
+      <c r="U17" s="95" t="s">
+        <v>376</v>
+      </c>
+      <c r="V17" s="95"/>
+      <c r="W17" s="83"/>
+    </row>
+    <row r="18" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A18" s="81"/>
+      <c r="B18" s="105"/>
+      <c r="C18" s="82" t="s">
+        <v>360</v>
+      </c>
+      <c r="D18" s="82" t="s">
+        <v>363</v>
+      </c>
+      <c r="E18" s="82"/>
+      <c r="F18" s="103"/>
+      <c r="G18" s="82"/>
+      <c r="H18" s="82"/>
+      <c r="I18" s="82"/>
+      <c r="J18" s="82"/>
+      <c r="K18" s="107" t="s">
+        <v>342</v>
+      </c>
+      <c r="L18" s="82" t="s">
+        <v>404</v>
+      </c>
+      <c r="M18" s="82"/>
+      <c r="N18" s="82"/>
+      <c r="O18" s="103"/>
+      <c r="P18" s="82"/>
+      <c r="Q18" s="82"/>
+      <c r="R18" s="82" t="s">
+        <v>377</v>
+      </c>
+      <c r="S18" s="82"/>
+      <c r="T18" s="82"/>
+      <c r="U18" s="82"/>
+      <c r="V18" s="82"/>
+      <c r="W18" s="83"/>
+    </row>
+    <row r="19" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="108"/>
+      <c r="C19" s="82" t="s">
+        <v>353</v>
+      </c>
+      <c r="D19" s="82" t="s">
+        <v>369</v>
+      </c>
+      <c r="E19" s="82"/>
+      <c r="F19" s="103"/>
+      <c r="G19" s="82"/>
+      <c r="H19" s="82"/>
+      <c r="I19" s="82"/>
+      <c r="J19" s="82"/>
+      <c r="K19" s="107" t="s">
+        <v>343</v>
+      </c>
+      <c r="L19" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="M19" s="82"/>
+      <c r="N19" s="82"/>
+      <c r="O19" s="103"/>
+      <c r="P19" s="82"/>
+      <c r="Q19" s="82"/>
+      <c r="R19" s="82"/>
+      <c r="S19" s="82"/>
+      <c r="T19" s="82"/>
+      <c r="U19" s="82"/>
+      <c r="V19" s="82"/>
+      <c r="W19" s="83"/>
+    </row>
+    <row r="20" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A20" s="81"/>
+      <c r="B20" s="107"/>
+      <c r="C20" s="82" t="s">
+        <v>361</v>
+      </c>
+      <c r="D20" s="82" t="s">
+        <v>362</v>
+      </c>
+      <c r="E20" s="82"/>
+      <c r="F20" s="103"/>
+      <c r="G20" s="82"/>
+      <c r="H20" s="82"/>
+      <c r="I20" s="82"/>
+      <c r="J20" s="82"/>
+      <c r="K20" s="107" t="s">
+        <v>367</v>
+      </c>
+      <c r="L20" s="82" t="s">
+        <v>406</v>
+      </c>
+      <c r="M20" s="82"/>
+      <c r="N20" s="82"/>
+      <c r="O20" s="103"/>
+      <c r="P20" s="82"/>
+      <c r="Q20" s="82"/>
+      <c r="R20" s="101" t="s">
+        <v>388</v>
+      </c>
+      <c r="S20" s="82"/>
+      <c r="T20" s="82"/>
+      <c r="U20" s="82"/>
+      <c r="V20" s="82"/>
+      <c r="W20" s="83"/>
+    </row>
+    <row r="21" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A21" s="81"/>
+      <c r="B21" s="109"/>
+      <c r="C21" s="110"/>
+      <c r="D21" s="110"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="111"/>
+      <c r="G21" s="82"/>
+      <c r="H21" s="82"/>
+      <c r="I21" s="82"/>
+      <c r="J21" s="82"/>
+      <c r="K21" s="109" t="s">
+        <v>366</v>
+      </c>
+      <c r="L21" s="110">
+        <v>0</v>
+      </c>
+      <c r="M21" s="110"/>
+      <c r="N21" s="110"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="82"/>
+      <c r="Q21" s="82"/>
+      <c r="R21" s="39" t="s">
+        <v>375</v>
+      </c>
+      <c r="S21" s="39" t="s">
+        <v>389</v>
+      </c>
+      <c r="T21" s="39" t="s">
+        <v>390</v>
+      </c>
+      <c r="U21" s="39" t="s">
+        <v>391</v>
+      </c>
+      <c r="V21" s="39" t="s">
+        <v>390</v>
+      </c>
+      <c r="W21" s="83"/>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A22" s="81"/>
+      <c r="B22" s="82"/>
+      <c r="C22" s="82"/>
+      <c r="D22" s="82"/>
+      <c r="E22" s="82"/>
+      <c r="F22" s="82"/>
+      <c r="G22" s="82"/>
+      <c r="H22" s="82"/>
+      <c r="I22" s="82"/>
+      <c r="J22" s="82"/>
+      <c r="K22" s="82"/>
+      <c r="L22" s="82"/>
+      <c r="M22" s="82"/>
+      <c r="N22" s="82"/>
+      <c r="O22" s="82"/>
+      <c r="P22" s="82"/>
+      <c r="Q22" s="82"/>
+      <c r="R22" s="95" t="s">
+        <v>396</v>
+      </c>
+      <c r="S22" s="95" t="s">
+        <v>392</v>
+      </c>
+      <c r="T22" s="95" t="s">
+        <v>393</v>
+      </c>
+      <c r="U22" s="95" t="s">
+        <v>357</v>
+      </c>
+      <c r="V22" s="95" t="s">
+        <v>394</v>
+      </c>
+      <c r="W22" s="83"/>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A23" s="81"/>
+      <c r="B23" s="112" t="s">
+        <v>355</v>
+      </c>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="93"/>
+      <c r="J23" s="82"/>
+      <c r="K23" s="98" t="s">
+        <v>347</v>
+      </c>
+      <c r="L23" s="99" t="s">
+        <v>350</v>
+      </c>
+      <c r="M23" s="99"/>
+      <c r="N23" s="99"/>
+      <c r="O23" s="100"/>
+      <c r="P23" s="82"/>
+      <c r="Q23" s="82"/>
+      <c r="R23" s="82" t="s">
+        <v>377</v>
+      </c>
+      <c r="S23" s="82"/>
+      <c r="T23" s="82"/>
+      <c r="U23" s="82"/>
+      <c r="V23" s="82"/>
+      <c r="W23" s="83"/>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A24" s="81"/>
+      <c r="B24" s="98" t="s">
+        <v>143</v>
+      </c>
+      <c r="C24" s="99" t="s">
+        <v>354</v>
+      </c>
+      <c r="D24" s="99"/>
+      <c r="E24" s="99" t="s">
+        <v>139</v>
+      </c>
+      <c r="F24" s="114" t="s">
+        <v>384</v>
+      </c>
+      <c r="G24" s="99"/>
+      <c r="H24" s="99"/>
+      <c r="I24" s="100"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="107"/>
+      <c r="L24" s="82" t="s">
+        <v>359</v>
+      </c>
+      <c r="M24" s="82"/>
+      <c r="N24" s="82"/>
+      <c r="O24" s="103"/>
+      <c r="P24" s="82"/>
+      <c r="Q24" s="82"/>
+      <c r="R24" s="82"/>
+      <c r="S24" s="82"/>
+      <c r="T24" s="82"/>
+      <c r="U24" s="82"/>
+      <c r="V24" s="82"/>
+      <c r="W24" s="83"/>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A25" s="81"/>
+      <c r="B25" s="107" t="s">
+        <v>345</v>
+      </c>
+      <c r="C25" s="82" t="s">
+        <v>351</v>
+      </c>
+      <c r="D25" s="82"/>
+      <c r="E25" s="82" t="s">
+        <v>144</v>
+      </c>
+      <c r="F25" s="82" t="s">
+        <v>385</v>
+      </c>
+      <c r="G25" s="82"/>
+      <c r="H25" s="82"/>
+      <c r="I25" s="103"/>
+      <c r="J25" s="82"/>
+      <c r="K25" s="107" t="s">
+        <v>342</v>
+      </c>
+      <c r="L25" s="82" t="s">
+        <v>407</v>
+      </c>
+      <c r="M25" s="82"/>
+      <c r="N25" s="82"/>
+      <c r="O25" s="103"/>
+      <c r="P25" s="82"/>
+      <c r="Q25" s="82"/>
+      <c r="R25" s="82"/>
+      <c r="S25" s="82"/>
+      <c r="T25" s="82"/>
+      <c r="U25" s="82"/>
+      <c r="V25" s="82"/>
+      <c r="W25" s="83"/>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A26" s="81"/>
+      <c r="B26" s="107" t="s">
+        <v>141</v>
+      </c>
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="82" t="s">
+        <v>346</v>
+      </c>
+      <c r="F26" s="106" t="s">
+        <v>386</v>
+      </c>
+      <c r="G26" s="82"/>
+      <c r="H26" s="82"/>
+      <c r="I26" s="103"/>
+      <c r="J26" s="82"/>
+      <c r="K26" s="107" t="s">
+        <v>343</v>
+      </c>
+      <c r="L26" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="M26" s="82"/>
+      <c r="N26" s="82"/>
+      <c r="O26" s="103"/>
+      <c r="P26" s="82"/>
+      <c r="Q26" s="82"/>
+      <c r="R26" s="82"/>
+      <c r="S26" s="82"/>
+      <c r="T26" s="82"/>
+      <c r="U26" s="82"/>
+      <c r="V26" s="82"/>
+      <c r="W26" s="83"/>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A27" s="81"/>
+      <c r="B27" s="107"/>
+      <c r="C27" s="98"/>
+      <c r="D27" s="99"/>
+      <c r="E27" s="99"/>
+      <c r="F27" s="100"/>
+      <c r="G27" s="82"/>
+      <c r="H27" s="82"/>
+      <c r="I27" s="103"/>
+      <c r="J27" s="82"/>
+      <c r="K27" s="107" t="s">
+        <v>367</v>
+      </c>
+      <c r="L27" s="82" t="s">
+        <v>408</v>
+      </c>
+      <c r="M27" s="82"/>
+      <c r="N27" s="82"/>
+      <c r="O27" s="103"/>
+      <c r="P27" s="82"/>
+      <c r="Q27" s="82"/>
+      <c r="R27" s="82"/>
+      <c r="S27" s="82"/>
+      <c r="T27" s="82"/>
+      <c r="U27" s="82"/>
+      <c r="V27" s="82"/>
+      <c r="W27" s="83"/>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A28" s="81"/>
+      <c r="B28" s="107"/>
+      <c r="C28" s="109"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="111"/>
+      <c r="G28" s="82"/>
+      <c r="H28" s="82"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="82"/>
+      <c r="K28" s="109" t="s">
+        <v>366</v>
+      </c>
+      <c r="L28" s="115">
+        <v>0</v>
+      </c>
+      <c r="M28" s="110"/>
+      <c r="N28" s="110"/>
+      <c r="O28" s="111"/>
+      <c r="P28" s="82"/>
+      <c r="Q28" s="82"/>
+      <c r="R28" s="82"/>
+      <c r="S28" s="82"/>
+      <c r="T28" s="82"/>
+      <c r="U28" s="82"/>
+      <c r="V28" s="82"/>
+      <c r="W28" s="83"/>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A29" s="81"/>
+      <c r="B29" s="107"/>
+      <c r="C29" s="82"/>
+      <c r="D29" s="82"/>
+      <c r="E29" s="82"/>
+      <c r="F29" s="82"/>
+      <c r="G29" s="82"/>
+      <c r="H29" s="82"/>
+      <c r="I29" s="103"/>
+      <c r="J29" s="82"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="82"/>
+      <c r="M29" s="82"/>
+      <c r="N29" s="82"/>
+      <c r="O29" s="82"/>
+      <c r="P29" s="82"/>
+      <c r="Q29" s="82"/>
+      <c r="R29" s="82"/>
+      <c r="S29" s="82"/>
+      <c r="T29" s="82"/>
+      <c r="U29" s="82"/>
+      <c r="V29" s="82"/>
+      <c r="W29" s="83"/>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A30" s="81"/>
+      <c r="B30" s="107" t="s">
+        <v>348</v>
+      </c>
+      <c r="C30" s="92" t="s">
+        <v>369</v>
+      </c>
+      <c r="D30" s="93"/>
+      <c r="E30" s="82"/>
+      <c r="F30" s="82"/>
+      <c r="G30" s="82" t="s">
+        <v>361</v>
+      </c>
+      <c r="H30" s="92" t="s">
+        <v>362</v>
+      </c>
+      <c r="I30" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="J30" s="82"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="82"/>
+      <c r="M30" s="82"/>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82"/>
+      <c r="P30" s="82"/>
+      <c r="Q30" s="82"/>
+      <c r="R30" s="82"/>
+      <c r="S30" s="82"/>
+      <c r="T30" s="82"/>
+      <c r="U30" s="82"/>
+      <c r="V30" s="82"/>
+      <c r="W30" s="83"/>
+    </row>
+    <row r="31" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A31" s="81"/>
+      <c r="B31" s="107"/>
+      <c r="C31" s="92" t="s">
+        <v>356</v>
+      </c>
+      <c r="D31" s="113"/>
+      <c r="E31" s="93"/>
+      <c r="F31" s="82"/>
+      <c r="G31" s="82" t="s">
+        <v>365</v>
+      </c>
+      <c r="H31" s="92" t="s">
+        <v>363</v>
+      </c>
+      <c r="I31" s="116" t="s">
+        <v>399</v>
+      </c>
+      <c r="J31" s="82"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="82"/>
+      <c r="M31" s="82"/>
+      <c r="N31" s="82"/>
+      <c r="O31" s="82"/>
+      <c r="P31" s="82"/>
+      <c r="Q31" s="82"/>
+      <c r="R31" s="82"/>
+      <c r="S31" s="82"/>
+      <c r="T31" s="82"/>
+      <c r="U31" s="82"/>
+      <c r="V31" s="82"/>
+      <c r="W31" s="83"/>
+    </row>
+    <row r="32" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A32" s="81"/>
+      <c r="B32" s="107" t="s">
+        <v>342</v>
+      </c>
+      <c r="C32" s="108" t="s">
+        <v>409</v>
+      </c>
+      <c r="D32" s="82"/>
+      <c r="E32" s="82"/>
+      <c r="F32" s="82"/>
+      <c r="G32" s="82"/>
+      <c r="H32" s="82"/>
+      <c r="I32" s="103"/>
+      <c r="J32" s="82"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="82"/>
+      <c r="M32" s="82"/>
+      <c r="N32" s="82"/>
+      <c r="O32" s="82"/>
+      <c r="P32" s="82"/>
+      <c r="Q32" s="82"/>
+      <c r="R32" s="82"/>
+      <c r="S32" s="82"/>
+      <c r="T32" s="82"/>
+      <c r="U32" s="82"/>
+      <c r="V32" s="82"/>
+      <c r="W32" s="83"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A33" s="81"/>
+      <c r="B33" s="107" t="s">
+        <v>343</v>
+      </c>
+      <c r="C33" s="95" t="s">
+        <v>410</v>
+      </c>
+      <c r="D33" s="82"/>
+      <c r="E33" s="82"/>
+      <c r="F33" s="82"/>
+      <c r="G33" s="82"/>
+      <c r="H33" s="82"/>
+      <c r="I33" s="103"/>
+      <c r="J33" s="82"/>
+      <c r="K33" s="82"/>
+      <c r="L33" s="82"/>
+      <c r="M33" s="82"/>
+      <c r="N33" s="82"/>
+      <c r="O33" s="82"/>
+      <c r="P33" s="82"/>
+      <c r="Q33" s="82"/>
+      <c r="R33" s="82"/>
+      <c r="S33" s="82"/>
+      <c r="T33" s="82"/>
+      <c r="U33" s="82"/>
+      <c r="V33" s="82"/>
+      <c r="W33" s="83"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A34" s="81"/>
+      <c r="B34" s="107"/>
+      <c r="C34" s="82"/>
+      <c r="D34" s="82"/>
+      <c r="E34" s="82"/>
+      <c r="F34" s="82"/>
+      <c r="G34" s="82"/>
+      <c r="H34" s="82"/>
+      <c r="I34" s="103"/>
+      <c r="J34" s="82"/>
+      <c r="K34" s="82"/>
+      <c r="L34" s="82"/>
+      <c r="M34" s="82"/>
+      <c r="N34" s="82"/>
+      <c r="O34" s="82"/>
+      <c r="P34" s="82"/>
+      <c r="Q34" s="82"/>
+      <c r="R34" s="82"/>
+      <c r="S34" s="82"/>
+      <c r="T34" s="82"/>
+      <c r="U34" s="82"/>
+      <c r="V34" s="82"/>
+      <c r="W34" s="83"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A35" s="81"/>
+      <c r="B35" s="107"/>
+      <c r="C35" s="82"/>
+      <c r="D35" s="82"/>
+      <c r="E35" s="82"/>
+      <c r="F35" s="82"/>
+      <c r="G35" s="82"/>
+      <c r="H35" s="82"/>
+      <c r="I35" s="103"/>
+      <c r="J35" s="82"/>
+      <c r="K35" s="82"/>
+      <c r="L35" s="82"/>
+      <c r="M35" s="82"/>
+      <c r="N35" s="82"/>
+      <c r="O35" s="82"/>
+      <c r="P35" s="82"/>
+      <c r="Q35" s="82"/>
+      <c r="R35" s="82"/>
+      <c r="S35" s="82"/>
+      <c r="T35" s="82"/>
+      <c r="U35" s="82"/>
+      <c r="V35" s="82"/>
+      <c r="W35" s="83"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A36" s="81"/>
+      <c r="B36" s="107"/>
+      <c r="C36" s="82"/>
+      <c r="D36" s="82"/>
+      <c r="E36" s="82"/>
+      <c r="F36" s="82"/>
+      <c r="G36" s="82"/>
+      <c r="H36" s="82"/>
+      <c r="I36" s="103"/>
+      <c r="J36" s="82"/>
+      <c r="K36" s="82"/>
+      <c r="L36" s="82"/>
+      <c r="M36" s="82"/>
+      <c r="N36" s="82"/>
+      <c r="O36" s="82"/>
+      <c r="P36" s="82"/>
+      <c r="Q36" s="82"/>
+      <c r="R36" s="82"/>
+      <c r="S36" s="82"/>
+      <c r="T36" s="82"/>
+      <c r="U36" s="82"/>
+      <c r="V36" s="82"/>
+      <c r="W36" s="83"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A37" s="81"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="110"/>
+      <c r="D37" s="110"/>
+      <c r="E37" s="110"/>
+      <c r="F37" s="110"/>
+      <c r="G37" s="110"/>
+      <c r="H37" s="110"/>
+      <c r="I37" s="111"/>
+      <c r="J37" s="82"/>
+      <c r="K37" s="82"/>
+      <c r="L37" s="82"/>
+      <c r="M37" s="82"/>
+      <c r="N37" s="82"/>
+      <c r="O37" s="82"/>
+      <c r="P37" s="82"/>
+      <c r="Q37" s="82"/>
+      <c r="R37" s="82"/>
+      <c r="S37" s="82"/>
+      <c r="T37" s="82"/>
+      <c r="U37" s="82"/>
+      <c r="V37" s="82"/>
+      <c r="W37" s="83"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="A38" s="81"/>
+      <c r="B38" s="82"/>
+      <c r="C38" s="82"/>
+      <c r="D38" s="82"/>
+      <c r="E38" s="82"/>
+      <c r="F38" s="82"/>
+      <c r="G38" s="82"/>
+      <c r="H38" s="82"/>
+      <c r="I38" s="82"/>
+      <c r="J38" s="82"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="82"/>
+      <c r="M38" s="82"/>
+      <c r="N38" s="82"/>
+      <c r="O38" s="82"/>
+      <c r="P38" s="82"/>
+      <c r="Q38" s="82"/>
+      <c r="R38" s="82"/>
+      <c r="S38" s="82"/>
+      <c r="T38" s="82"/>
+      <c r="U38" s="82"/>
+      <c r="V38" s="82"/>
+      <c r="W38" s="83"/>
+    </row>
+    <row r="39" spans="1:23" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="117"/>
+      <c r="B39" s="118"/>
+      <c r="C39" s="118"/>
+      <c r="D39" s="118"/>
+      <c r="E39" s="118"/>
+      <c r="F39" s="118"/>
+      <c r="G39" s="118"/>
+      <c r="H39" s="118"/>
+      <c r="I39" s="118"/>
+      <c r="J39" s="118"/>
+      <c r="K39" s="118"/>
+      <c r="L39" s="118"/>
+      <c r="M39" s="118"/>
+      <c r="N39" s="118"/>
+      <c r="O39" s="118"/>
+      <c r="P39" s="118"/>
+      <c r="Q39" s="118"/>
+      <c r="R39" s="118"/>
+      <c r="S39" s="118"/>
+      <c r="T39" s="118"/>
+      <c r="U39" s="118"/>
+      <c r="V39" s="118"/>
+      <c r="W39" s="119"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B43" s="148" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="149"/>
+      <c r="D43" s="149"/>
+      <c r="E43" s="149"/>
+      <c r="F43" s="149"/>
+      <c r="G43" s="149"/>
+      <c r="H43" s="150"/>
+      <c r="K43" s="123" t="s">
+        <v>7</v>
+      </c>
+      <c r="L43" s="42"/>
+      <c r="M43" s="42"/>
+      <c r="N43" s="42"/>
+      <c r="O43" s="42"/>
+      <c r="P43" s="42"/>
+      <c r="Q43" s="43"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B44" s="124" t="s">
         <v>411</v>
       </c>
-    </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B3" s="24" t="s">
-        <v>339</v>
-      </c>
-      <c r="C3" s="45" t="s">
-        <v>340</v>
-      </c>
-      <c r="E3" s="45" t="s">
-        <v>341</v>
-      </c>
-      <c r="G3" s="45" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="4" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="104" t="s">
-        <v>380</v>
-      </c>
-      <c r="C4" s="105"/>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="106"/>
-    </row>
-    <row r="5" spans="1:22" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="107" t="s">
-        <v>381</v>
-      </c>
-      <c r="C5" s="108"/>
-      <c r="D5" s="108"/>
-      <c r="E5" s="108"/>
-      <c r="F5" s="109"/>
-    </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>138</v>
-      </c>
-      <c r="C7" t="s">
-        <v>379</v>
-      </c>
-      <c r="G7" t="s">
-        <v>137</v>
-      </c>
-      <c r="H7" t="s">
-        <v>382</v>
-      </c>
-    </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="G8" t="s">
-        <v>139</v>
-      </c>
-      <c r="H8" s="110" t="s">
-        <v>383</v>
-      </c>
-    </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="C9" t="s">
-        <v>342</v>
-      </c>
-      <c r="D9" t="s">
-        <v>407</v>
-      </c>
-      <c r="E9" t="s">
-        <v>343</v>
-      </c>
-      <c r="F9" t="s">
-        <v>405</v>
-      </c>
-      <c r="G9" t="s">
-        <v>344</v>
-      </c>
-      <c r="H9" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>140</v>
-      </c>
-      <c r="C10" t="s">
-        <v>384</v>
-      </c>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B13" s="88" t="s">
-        <v>142</v>
-      </c>
-      <c r="C13" s="85" t="s">
-        <v>369</v>
-      </c>
-      <c r="D13" s="86"/>
-      <c r="E13" s="87" t="s">
-        <v>372</v>
-      </c>
-      <c r="F13" s="87" t="s">
+      <c r="C44" s="146" t="s">
+        <v>419</v>
+      </c>
+      <c r="D44" s="147"/>
+      <c r="E44" s="125"/>
+      <c r="F44" s="125"/>
+      <c r="G44" s="125"/>
+      <c r="H44" s="126"/>
+      <c r="K44" s="50"/>
+      <c r="L44" s="48"/>
+      <c r="M44" s="48"/>
+      <c r="N44" s="48"/>
+      <c r="O44" s="48"/>
+      <c r="P44" s="48"/>
+      <c r="Q44" s="49"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B45" s="127"/>
+      <c r="C45" s="128"/>
+      <c r="D45" s="128"/>
+      <c r="E45" s="128"/>
+      <c r="F45" s="128"/>
+      <c r="G45" s="128"/>
+      <c r="H45" s="126"/>
+      <c r="K45" s="50" t="s">
+        <v>411</v>
+      </c>
+      <c r="L45" s="48" t="s">
+        <v>436</v>
+      </c>
+      <c r="M45" s="48"/>
+      <c r="N45" s="48"/>
+      <c r="O45" s="48"/>
+      <c r="P45" s="48"/>
+      <c r="Q45" s="49"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B46" s="129" t="s">
+        <v>389</v>
+      </c>
+      <c r="C46" s="130" t="s">
+        <v>421</v>
+      </c>
+      <c r="D46" s="130"/>
+      <c r="E46" s="131" t="s">
+        <v>391</v>
+      </c>
+      <c r="F46" s="130" t="s">
+        <v>420</v>
+      </c>
+      <c r="G46" s="130"/>
+      <c r="H46" s="126"/>
+      <c r="K46" s="50" t="s">
+        <v>422</v>
+      </c>
+      <c r="L46" s="48" t="s">
+        <v>437</v>
+      </c>
+      <c r="M46" s="48"/>
+      <c r="N46" s="48"/>
+      <c r="O46" s="48"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="49"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B47" s="129" t="s">
+        <v>413</v>
+      </c>
+      <c r="C47" s="130" t="s">
+        <v>393</v>
+      </c>
+      <c r="D47" s="130"/>
+      <c r="E47" s="131" t="s">
+        <v>412</v>
+      </c>
+      <c r="F47" s="130" t="s">
+        <v>416</v>
+      </c>
+      <c r="G47" s="130"/>
+      <c r="H47" s="126"/>
+      <c r="K47" s="159" t="s">
+        <v>432</v>
+      </c>
+      <c r="L47" s="153" t="s">
+        <v>433</v>
+      </c>
+      <c r="M47" s="154">
+        <v>44530</v>
+      </c>
+      <c r="N47" s="155"/>
+      <c r="O47" s="48"/>
+      <c r="P47" s="48"/>
+      <c r="Q47" s="49"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="B48" s="129" t="s">
+        <v>366</v>
+      </c>
+      <c r="C48" s="130">
+        <v>0</v>
+      </c>
+      <c r="D48" s="130"/>
+      <c r="E48" s="131" t="s">
+        <v>366</v>
+      </c>
+      <c r="F48" s="130">
+        <v>0</v>
+      </c>
+      <c r="G48" s="130"/>
+      <c r="H48" s="126"/>
+      <c r="K48" s="50"/>
+      <c r="L48" s="48"/>
+      <c r="M48" s="48"/>
+      <c r="N48" s="48"/>
+      <c r="O48" s="48"/>
+      <c r="P48" s="48"/>
+      <c r="Q48" s="49"/>
+    </row>
+    <row r="49" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B49" s="129" t="s">
+        <v>415</v>
+      </c>
+      <c r="C49" s="130" t="s">
+        <v>417</v>
+      </c>
+      <c r="D49" s="130"/>
+      <c r="E49" s="125"/>
+      <c r="F49" s="125"/>
+      <c r="G49" s="125"/>
+      <c r="H49" s="126"/>
+      <c r="K49" s="50"/>
+      <c r="L49" s="48"/>
+      <c r="M49" s="48"/>
+      <c r="N49" s="48"/>
+      <c r="O49" s="48"/>
+      <c r="P49" s="48"/>
+      <c r="Q49" s="49"/>
+      <c r="R49" s="19"/>
+      <c r="S49" s="121"/>
+      <c r="T49" s="121"/>
+      <c r="U49" s="19"/>
+      <c r="V49" s="19"/>
+      <c r="W49" s="19"/>
+      <c r="X49" s="19"/>
+    </row>
+    <row r="50" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B50" s="129" t="s">
+        <v>414</v>
+      </c>
+      <c r="C50" s="130">
+        <v>10500</v>
+      </c>
+      <c r="D50" s="130"/>
+      <c r="E50" s="125"/>
+      <c r="F50" s="125"/>
+      <c r="G50" s="125"/>
+      <c r="H50" s="126"/>
+      <c r="K50" s="156" t="s">
+        <v>431</v>
+      </c>
+      <c r="L50" s="157"/>
+      <c r="M50" s="157"/>
+      <c r="N50" s="157"/>
+      <c r="O50" s="157"/>
+      <c r="P50" s="157"/>
+      <c r="Q50" s="158"/>
+      <c r="S50" s="120"/>
+      <c r="T50" s="120"/>
+      <c r="W50" s="151"/>
+      <c r="X50" s="151"/>
+    </row>
+    <row r="51" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B51" s="132" t="s">
         <v>141</v>
       </c>
-      <c r="K13" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="L13" s="97" t="s">
-        <v>369</v>
-      </c>
-      <c r="M13" s="98"/>
-      <c r="N13" s="87" t="s">
-        <v>372</v>
-      </c>
-      <c r="O13" s="87" t="s">
-        <v>141</v>
-      </c>
-      <c r="R13" s="90" t="s">
-        <v>142</v>
-      </c>
-      <c r="S13" s="99" t="s">
-        <v>369</v>
-      </c>
-      <c r="T13" s="100"/>
-      <c r="U13" s="96" t="s">
-        <v>372</v>
-      </c>
-      <c r="V13" s="87" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="K14" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="R14" s="101"/>
-      <c r="S14" s="101"/>
-      <c r="T14" s="101"/>
-      <c r="U14" s="101"/>
-      <c r="V14" s="101"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B15" s="46"/>
-      <c r="C15" s="47" t="s">
-        <v>355</v>
-      </c>
-      <c r="D15" s="47"/>
-      <c r="E15" s="47"/>
-      <c r="F15" s="48"/>
-      <c r="R15" s="102" t="s">
-        <v>373</v>
-      </c>
-      <c r="S15" s="101"/>
-      <c r="T15" s="101"/>
-      <c r="U15" s="101"/>
-      <c r="V15" s="101"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="B16" s="76"/>
-      <c r="C16" s="79" t="s">
-        <v>352</v>
-      </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="80"/>
-      <c r="K16" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="L16" s="47" t="s">
-        <v>349</v>
-      </c>
-      <c r="M16" s="47"/>
-      <c r="N16" s="47"/>
-      <c r="O16" s="48"/>
-      <c r="R16" s="42" t="s">
-        <v>80</v>
-      </c>
-      <c r="S16" s="42" t="s">
-        <v>72</v>
-      </c>
-      <c r="T16" s="42" t="s">
-        <v>375</v>
-      </c>
-      <c r="U16" s="42" t="s">
-        <v>374</v>
-      </c>
-      <c r="V16" s="42" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="77"/>
-      <c r="C17" s="81" t="s">
-        <v>353</v>
-      </c>
-      <c r="D17" s="79"/>
-      <c r="E17" s="79"/>
-      <c r="F17" s="80"/>
-      <c r="K17" s="82"/>
-      <c r="L17" s="79" t="s">
-        <v>359</v>
-      </c>
-      <c r="M17" s="79"/>
-      <c r="N17" s="79"/>
-      <c r="O17" s="80"/>
-      <c r="R17" s="6" t="s">
-        <v>396</v>
-      </c>
-      <c r="S17" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="T17" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="U17" s="6" t="s">
-        <v>377</v>
-      </c>
-      <c r="V17" s="6"/>
-    </row>
-    <row r="18" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B18" s="77"/>
-      <c r="C18" s="79" t="s">
-        <v>361</v>
-      </c>
-      <c r="D18" s="79" t="s">
-        <v>364</v>
-      </c>
-      <c r="E18" s="79"/>
-      <c r="F18" s="80"/>
-      <c r="K18" s="82" t="s">
-        <v>342</v>
-      </c>
-      <c r="L18" s="89" t="s">
-        <v>402</v>
-      </c>
-      <c r="M18" s="79"/>
-      <c r="N18" s="79"/>
-      <c r="O18" s="80"/>
-      <c r="R18" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="19" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B19" s="78"/>
-      <c r="C19" s="79" t="s">
-        <v>354</v>
-      </c>
-      <c r="D19" s="79" t="s">
-        <v>370</v>
-      </c>
-      <c r="E19" s="79"/>
-      <c r="F19" s="80"/>
-      <c r="K19" s="82" t="s">
-        <v>343</v>
-      </c>
-      <c r="L19" s="89" t="s">
-        <v>400</v>
-      </c>
-      <c r="M19" s="79"/>
-      <c r="N19" s="79"/>
-      <c r="O19" s="80"/>
-    </row>
-    <row r="20" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B20" s="82"/>
-      <c r="C20" s="89" t="s">
-        <v>362</v>
-      </c>
-      <c r="D20" s="79" t="s">
-        <v>363</v>
-      </c>
-      <c r="E20" s="79"/>
-      <c r="F20" s="80"/>
-      <c r="K20" s="91" t="s">
-        <v>368</v>
-      </c>
-      <c r="L20" s="89" t="s">
-        <v>401</v>
-      </c>
-      <c r="M20" s="79"/>
-      <c r="N20" s="79"/>
-      <c r="O20" s="80"/>
-      <c r="R20" s="102" t="s">
-        <v>389</v>
-      </c>
-      <c r="S20" s="101"/>
-      <c r="T20" s="101"/>
-      <c r="U20" s="101"/>
-      <c r="V20" s="101"/>
-    </row>
-    <row r="21" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B21" s="49"/>
-      <c r="C21" s="50"/>
-      <c r="D21" s="50"/>
-      <c r="E21" s="50"/>
-      <c r="F21" s="51"/>
-      <c r="K21" s="92" t="s">
-        <v>367</v>
-      </c>
-      <c r="L21" s="50">
+      <c r="C51" s="133"/>
+      <c r="D51" s="133"/>
+      <c r="E51" s="125"/>
+      <c r="F51" s="125"/>
+      <c r="G51" s="125"/>
+      <c r="H51" s="126"/>
+      <c r="K51" s="47" t="s">
+        <v>423</v>
+      </c>
+      <c r="L51" s="6" t="s">
+        <v>428</v>
+      </c>
+      <c r="M51" s="6" t="s">
+        <v>434</v>
+      </c>
+      <c r="N51" s="47" t="s">
+        <v>430</v>
+      </c>
+      <c r="O51" s="47" t="s">
+        <v>424</v>
+      </c>
+      <c r="P51" s="47" t="s">
+        <v>425</v>
+      </c>
+      <c r="Q51" s="49"/>
+    </row>
+    <row r="52" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B52" s="134" t="s">
+        <v>418</v>
+      </c>
+      <c r="C52" s="135"/>
+      <c r="D52" s="135"/>
+      <c r="E52" s="135"/>
+      <c r="F52" s="135"/>
+      <c r="G52" s="136"/>
+      <c r="H52" s="126"/>
+      <c r="K52" s="6" t="s">
+        <v>427</v>
+      </c>
+      <c r="L52" s="6" t="s">
+        <v>429</v>
+      </c>
+      <c r="M52" s="6" t="s">
+        <v>435</v>
+      </c>
+      <c r="N52" s="6">
+        <v>1000</v>
+      </c>
+      <c r="O52" s="6">
+        <v>2</v>
+      </c>
+      <c r="P52" s="6">
         <v>0</v>
       </c>
-      <c r="M21" s="50"/>
-      <c r="N21" s="50"/>
-      <c r="O21" s="51"/>
-      <c r="R21" s="43" t="s">
-        <v>376</v>
-      </c>
-      <c r="S21" s="43" t="s">
-        <v>390</v>
-      </c>
-      <c r="T21" s="43" t="s">
-        <v>391</v>
-      </c>
-      <c r="U21" s="43" t="s">
-        <v>392</v>
-      </c>
-      <c r="V21" s="43" t="s">
-        <v>391</v>
-      </c>
-    </row>
-    <row r="22" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="R22" s="6" t="s">
-        <v>397</v>
-      </c>
-      <c r="S22" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="T22" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="U22" s="6" t="s">
-        <v>358</v>
-      </c>
-      <c r="V22" s="6" t="s">
-        <v>395</v>
-      </c>
-    </row>
-    <row r="23" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B23" s="94" t="s">
-        <v>356</v>
-      </c>
-      <c r="C23" s="103"/>
-      <c r="D23" s="103"/>
-      <c r="E23" s="103"/>
-      <c r="F23" s="103"/>
-      <c r="G23" s="103"/>
-      <c r="H23" s="103"/>
-      <c r="I23" s="95"/>
-      <c r="K23" s="46" t="s">
-        <v>347</v>
-      </c>
-      <c r="L23" s="47" t="s">
-        <v>351</v>
-      </c>
-      <c r="M23" s="47"/>
-      <c r="N23" s="47"/>
-      <c r="O23" s="48"/>
-      <c r="R23" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="24" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B24" s="46" t="s">
-        <v>143</v>
-      </c>
-      <c r="C24" s="47" t="s">
-        <v>355</v>
-      </c>
-      <c r="D24" s="47"/>
-      <c r="E24" s="47" t="s">
-        <v>139</v>
-      </c>
-      <c r="F24" s="111" t="s">
-        <v>385</v>
-      </c>
-      <c r="G24" s="47"/>
-      <c r="H24" s="47"/>
-      <c r="I24" s="48"/>
-      <c r="K24" s="82"/>
-      <c r="L24" s="79" t="s">
-        <v>360</v>
-      </c>
-      <c r="M24" s="79"/>
-      <c r="N24" s="79"/>
-      <c r="O24" s="80"/>
-    </row>
-    <row r="25" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B25" s="82" t="s">
-        <v>345</v>
-      </c>
-      <c r="C25" s="79" t="s">
-        <v>352</v>
-      </c>
-      <c r="D25" s="79"/>
-      <c r="E25" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="F25" s="89" t="s">
-        <v>386</v>
-      </c>
-      <c r="G25" s="79"/>
-      <c r="H25" s="79"/>
-      <c r="I25" s="80"/>
-      <c r="K25" s="82" t="s">
-        <v>342</v>
-      </c>
-      <c r="L25" s="89" t="s">
-        <v>403</v>
-      </c>
-      <c r="M25" s="79"/>
-      <c r="N25" s="79"/>
-      <c r="O25" s="80"/>
-    </row>
-    <row r="26" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B26" s="82" t="s">
-        <v>141</v>
-      </c>
-      <c r="C26" s="79"/>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79" t="s">
-        <v>346</v>
-      </c>
-      <c r="F26" s="81" t="s">
-        <v>387</v>
-      </c>
-      <c r="G26" s="79"/>
-      <c r="H26" s="79"/>
-      <c r="I26" s="80"/>
-      <c r="K26" s="82" t="s">
-        <v>343</v>
-      </c>
-      <c r="L26" s="79" t="s">
-        <v>400</v>
-      </c>
-      <c r="M26" s="79"/>
-      <c r="N26" s="79"/>
-      <c r="O26" s="80"/>
-    </row>
-    <row r="27" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B27" s="82"/>
-      <c r="C27" s="46"/>
-      <c r="D27" s="47"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="48"/>
-      <c r="G27" s="79"/>
-      <c r="H27" s="79"/>
-      <c r="I27" s="80"/>
-      <c r="K27" s="91" t="s">
-        <v>368</v>
-      </c>
-      <c r="L27" s="89" t="s">
-        <v>404</v>
-      </c>
-      <c r="M27" s="79"/>
-      <c r="N27" s="79"/>
-      <c r="O27" s="80"/>
-    </row>
-    <row r="28" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B28" s="82"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="50"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51"/>
-      <c r="G28" s="79"/>
-      <c r="H28" s="79"/>
-      <c r="I28" s="80"/>
-      <c r="K28" s="92" t="s">
-        <v>367</v>
-      </c>
-      <c r="L28" s="93">
-        <v>0</v>
-      </c>
-      <c r="M28" s="50"/>
-      <c r="N28" s="50"/>
-      <c r="O28" s="51"/>
-    </row>
-    <row r="29" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B29" s="82"/>
-      <c r="C29" s="79"/>
-      <c r="D29" s="79"/>
-      <c r="E29" s="79"/>
-      <c r="F29" s="79"/>
-      <c r="G29" s="79"/>
-      <c r="H29" s="79"/>
-      <c r="I29" s="80"/>
-    </row>
-    <row r="30" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B30" s="82" t="s">
-        <v>348</v>
-      </c>
-      <c r="C30" s="83" t="s">
-        <v>350</v>
-      </c>
-      <c r="D30" s="84"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79" t="s">
-        <v>362</v>
-      </c>
-      <c r="H30" s="83" t="s">
-        <v>363</v>
-      </c>
-      <c r="I30" s="112" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="31" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B31" s="82"/>
-      <c r="C31" s="83" t="s">
-        <v>357</v>
-      </c>
-      <c r="D31" s="47"/>
-      <c r="E31" s="84"/>
-      <c r="F31" s="89"/>
-      <c r="G31" s="79" t="s">
-        <v>366</v>
-      </c>
-      <c r="H31" s="83" t="s">
-        <v>364</v>
-      </c>
-      <c r="I31" s="112" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="32" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B32" s="82" t="s">
-        <v>342</v>
-      </c>
-      <c r="C32" s="6" t="s">
-        <v>409</v>
-      </c>
-      <c r="D32" s="79"/>
-      <c r="E32" s="79"/>
-      <c r="F32" s="89"/>
-      <c r="G32" s="79"/>
-      <c r="H32" s="79"/>
-      <c r="I32" s="80"/>
-    </row>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="82" t="s">
-        <v>343</v>
-      </c>
-      <c r="C33" s="6" t="s">
-        <v>410</v>
-      </c>
-      <c r="D33" s="79"/>
-      <c r="E33" s="79"/>
-      <c r="F33" s="79"/>
-      <c r="G33" s="79"/>
-      <c r="H33" s="79"/>
-      <c r="I33" s="80"/>
-    </row>
-    <row r="34" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B34" s="82"/>
-      <c r="C34" s="79"/>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="79"/>
-      <c r="H34" s="79"/>
-      <c r="I34" s="80"/>
-    </row>
-    <row r="35" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B35" s="82"/>
-      <c r="C35" s="79"/>
-      <c r="D35" s="79"/>
-      <c r="E35" s="79"/>
-      <c r="F35" s="79"/>
-      <c r="G35" s="79"/>
-      <c r="H35" s="79"/>
-      <c r="I35" s="80"/>
-    </row>
-    <row r="36" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B36" s="82"/>
-      <c r="C36" s="79"/>
-      <c r="D36" s="79"/>
-      <c r="E36" s="79"/>
-      <c r="F36" s="89"/>
-      <c r="G36" s="79"/>
-      <c r="H36" s="79"/>
-      <c r="I36" s="80"/>
-    </row>
-    <row r="37" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B37" s="49"/>
-      <c r="C37" s="50"/>
-      <c r="D37" s="50"/>
-      <c r="E37" s="50"/>
-      <c r="F37" s="50"/>
-      <c r="G37" s="50"/>
-      <c r="H37" s="50"/>
-      <c r="I37" s="51"/>
+      <c r="Q52" s="49"/>
+    </row>
+    <row r="53" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B53" s="137"/>
+      <c r="C53" s="138"/>
+      <c r="D53" s="138"/>
+      <c r="E53" s="138"/>
+      <c r="F53" s="138"/>
+      <c r="G53" s="139"/>
+      <c r="H53" s="126"/>
+      <c r="K53" s="71" t="s">
+        <v>426</v>
+      </c>
+      <c r="L53" s="71"/>
+      <c r="M53" s="71"/>
+      <c r="N53" s="71"/>
+      <c r="O53" s="71"/>
+      <c r="P53" s="71"/>
+      <c r="Q53" s="49"/>
+    </row>
+    <row r="54" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B54" s="137"/>
+      <c r="C54" s="138"/>
+      <c r="D54" s="138"/>
+      <c r="E54" s="138"/>
+      <c r="F54" s="138"/>
+      <c r="G54" s="139"/>
+      <c r="H54" s="126"/>
+      <c r="K54" s="50"/>
+      <c r="L54" s="48"/>
+      <c r="M54" s="48"/>
+      <c r="N54" s="48"/>
+      <c r="O54" s="48"/>
+      <c r="P54" s="48"/>
+      <c r="Q54" s="49"/>
+    </row>
+    <row r="55" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B55" s="140"/>
+      <c r="C55" s="141"/>
+      <c r="D55" s="141"/>
+      <c r="E55" s="141"/>
+      <c r="F55" s="141"/>
+      <c r="G55" s="142"/>
+      <c r="H55" s="126"/>
+      <c r="K55" s="44"/>
+      <c r="L55" s="45"/>
+      <c r="M55" s="45"/>
+      <c r="N55" s="45"/>
+      <c r="O55" s="45"/>
+      <c r="P55" s="45"/>
+      <c r="Q55" s="46"/>
+    </row>
+    <row r="56" spans="2:24" x14ac:dyDescent="0.25">
+      <c r="B56" s="143"/>
+      <c r="C56" s="144"/>
+      <c r="D56" s="144"/>
+      <c r="E56" s="144"/>
+      <c r="F56" s="144"/>
+      <c r="G56" s="144"/>
+      <c r="H56" s="145"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="21">
+    <mergeCell ref="B52:G55"/>
+    <mergeCell ref="B43:H43"/>
+    <mergeCell ref="S49:T49"/>
+    <mergeCell ref="S50:T50"/>
+    <mergeCell ref="K50:Q50"/>
+    <mergeCell ref="K53:P53"/>
+    <mergeCell ref="C51:D51"/>
+    <mergeCell ref="C50:D50"/>
+    <mergeCell ref="C49:D49"/>
+    <mergeCell ref="C48:D48"/>
+    <mergeCell ref="C47:D47"/>
     <mergeCell ref="S13:T13"/>
     <mergeCell ref="L13:M13"/>
     <mergeCell ref="B5:F5"/>
     <mergeCell ref="B4:F4"/>
+    <mergeCell ref="F48:G48"/>
+    <mergeCell ref="F47:G47"/>
+    <mergeCell ref="F46:G46"/>
+    <mergeCell ref="C46:D46"/>
+    <mergeCell ref="C44:D44"/>
+    <mergeCell ref="B45:G45"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="H8" r:id="rId1"/>
@@ -5550,29 +6779,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="52" t="s">
         <v>70</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="55"/>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="56"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54"/>
+      <c r="E2" s="54"/>
+      <c r="F2" s="54"/>
+      <c r="G2" s="54"/>
+      <c r="H2" s="54"/>
+      <c r="I2" s="55"/>
       <c r="J2" s="12" t="s">
         <v>71</v>
       </c>
@@ -5788,29 +7017,29 @@
       <c r="J9" s="15"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="57" t="s">
+      <c r="A13" s="56" t="s">
         <v>103</v>
       </c>
-      <c r="B13" s="57"/>
-      <c r="C13" s="57"/>
-      <c r="D13" s="58"/>
-      <c r="E13" s="58"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="58"/>
-      <c r="H13" s="58"/>
-      <c r="I13" s="58"/>
-      <c r="J13" s="58"/>
+      <c r="B13" s="56"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="57"/>
+      <c r="E13" s="57"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="57"/>
+      <c r="H13" s="57"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="57"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="52"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="52"/>
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="51"/>
+      <c r="E14" s="51"/>
+      <c r="F14" s="51"/>
+      <c r="G14" s="51"/>
+      <c r="H14" s="51"/>
+      <c r="I14" s="51"/>
       <c r="J14" s="17" t="s">
         <v>71</v>
       </c>
@@ -6381,18 +7610,18 @@
       <c r="B2" t="s">
         <v>30</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="56" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57" t="s">
+      <c r="E2" s="56"/>
+      <c r="F2" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57" t="s">
+      <c r="G2" s="56"/>
+      <c r="H2" s="56" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="57"/>
+      <c r="I2" s="56"/>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
@@ -6500,14 +7729,14 @@
       </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="E8" s="57"/>
-      <c r="F8" s="59"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="59"/>
-      <c r="I8" s="60"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="58"/>
+      <c r="I8" s="59"/>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="D9" s="6" t="s">
@@ -6604,8 +7833,8 @@
       </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="H14" s="59"/>
-      <c r="I14" s="60"/>
+      <c r="H14" s="58"/>
+      <c r="I14" s="59"/>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="H15" s="6" t="s">
@@ -6644,8 +7873,8 @@
       </c>
     </row>
     <row r="20" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H20" s="59"/>
-      <c r="I20" s="60"/>
+      <c r="H20" s="58"/>
+      <c r="I20" s="59"/>
     </row>
     <row r="21" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H21" s="6" t="s">
@@ -6684,8 +7913,8 @@
       </c>
     </row>
     <row r="26" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H26" s="59"/>
-      <c r="I26" s="60"/>
+      <c r="H26" s="58"/>
+      <c r="I26" s="59"/>
     </row>
     <row r="27" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H27" s="6" t="s">
@@ -6724,8 +7953,8 @@
       </c>
     </row>
     <row r="32" spans="8:9" x14ac:dyDescent="0.25">
-      <c r="H32" s="59"/>
-      <c r="I32" s="60"/>
+      <c r="H32" s="58"/>
+      <c r="I32" s="59"/>
     </row>
     <row r="33" spans="8:9" x14ac:dyDescent="0.25">
       <c r="H33" s="6" t="s">
@@ -6883,7 +8112,7 @@
       <c r="B12" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="60" t="s">
         <v>17</v>
       </c>
     </row>
@@ -6891,7 +8120,7 @@
       <c r="B13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="54"/>
+      <c r="C13" s="53"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
@@ -6905,7 +8134,7 @@
       <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="61" t="s">
+      <c r="C15" s="60" t="s">
         <v>19</v>
       </c>
     </row>
@@ -6913,7 +8142,7 @@
       <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="61"/>
+      <c r="C16" s="60"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -6931,10 +8160,10 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="61" t="s">
+      <c r="B21" s="60" t="s">
         <v>23</v>
       </c>
-      <c r="C21" s="61"/>
+      <c r="C21" s="60"/>
       <c r="F21" s="1"/>
     </row>
   </sheetData>
@@ -6956,7 +8185,7 @@
   <dimension ref="B1:AD19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R23" sqref="R23"/>
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6967,54 +8196,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B1" s="62" t="s">
+      <c r="B1" s="61" t="s">
         <v>198</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="61" t="s">
         <v>194</v>
       </c>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62" t="s">
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
+      <c r="F1" s="61"/>
+      <c r="G1" s="61" t="s">
         <v>195</v>
       </c>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62" t="s">
+      <c r="H1" s="61"/>
+      <c r="I1" s="61"/>
+      <c r="J1" s="61"/>
+      <c r="K1" s="61" t="s">
         <v>196</v>
       </c>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62" t="s">
+      <c r="L1" s="61"/>
+      <c r="M1" s="61"/>
+      <c r="N1" s="61"/>
+      <c r="O1" s="61" t="s">
         <v>200</v>
       </c>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62" t="s">
+      <c r="P1" s="61"/>
+      <c r="Q1" s="61"/>
+      <c r="R1" s="61"/>
+      <c r="S1" s="61" t="s">
         <v>203</v>
       </c>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62" t="s">
+      <c r="T1" s="61"/>
+      <c r="U1" s="61"/>
+      <c r="V1" s="61"/>
+      <c r="W1" s="61" t="s">
         <v>205</v>
       </c>
-      <c r="X1" s="62"/>
-      <c r="Y1" s="62"/>
-      <c r="Z1" s="62"/>
-      <c r="AA1" s="62" t="s">
+      <c r="X1" s="61"/>
+      <c r="Y1" s="61"/>
+      <c r="Z1" s="61"/>
+      <c r="AA1" s="61" t="s">
         <v>338</v>
       </c>
-      <c r="AB1" s="62"/>
-      <c r="AC1" s="62"/>
-      <c r="AD1" s="62"/>
+      <c r="AB1" s="61"/>
+      <c r="AC1" s="61"/>
+      <c r="AD1" s="61"/>
     </row>
     <row r="2" spans="2:30" x14ac:dyDescent="0.25">
-      <c r="B2" s="62"/>
+      <c r="B2" s="61"/>
       <c r="C2" s="25">
         <v>1</v>
       </c>
@@ -7578,12 +8807,12 @@
       <c r="L17" s="6"/>
       <c r="M17" s="6"/>
       <c r="N17" s="6"/>
-      <c r="O17" s="63" t="s">
+      <c r="O17" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="P17" s="64"/>
-      <c r="Q17" s="64"/>
-      <c r="R17" s="65"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="63"/>
+      <c r="R17" s="64"/>
       <c r="S17" s="30"/>
       <c r="T17" s="30"/>
       <c r="U17" s="30"/>
@@ -7684,8 +8913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:L64"/>
   <sheetViews>
-    <sheetView topLeftCell="C46" workbookViewId="0">
-      <selection activeCell="G49" sqref="G49"/>
+    <sheetView topLeftCell="C4" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7703,63 +8932,63 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="65" t="s">
         <v>207</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="65" t="s">
         <v>214</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="65" t="s">
         <v>216</v>
       </c>
       <c r="E2" s="40" t="s">
         <v>331</v>
       </c>
-      <c r="F2" s="74" t="s">
+      <c r="F2" s="65" t="s">
         <v>208</v>
       </c>
-      <c r="G2" s="74" t="s">
+      <c r="G2" s="65" t="s">
         <v>210</v>
       </c>
-      <c r="H2" s="74" t="s">
+      <c r="H2" s="65" t="s">
         <v>211</v>
       </c>
-      <c r="I2" s="74" t="s">
+      <c r="I2" s="65" t="s">
         <v>212</v>
       </c>
-      <c r="J2" s="74" t="s">
+      <c r="J2" s="65" t="s">
         <v>209</v>
       </c>
-      <c r="K2" s="74" t="s">
+      <c r="K2" s="65" t="s">
         <v>213</v>
       </c>
-      <c r="L2" s="74" t="s">
+      <c r="L2" s="65" t="s">
         <v>215</v>
       </c>
     </row>
     <row r="3" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B3" s="75"/>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
       <c r="E3" s="39" t="s">
         <v>332</v>
       </c>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
-      <c r="I3" s="75"/>
-      <c r="J3" s="75"/>
-      <c r="K3" s="75"/>
-      <c r="L3" s="75"/>
+      <c r="F3" s="66"/>
+      <c r="G3" s="66"/>
+      <c r="H3" s="66"/>
+      <c r="I3" s="66"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="66"/>
+      <c r="L3" s="66"/>
     </row>
     <row r="4" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="62">
+      <c r="B4" s="61">
         <v>1</v>
       </c>
-      <c r="C4" s="67" t="s">
+      <c r="C4" s="70" t="s">
         <v>184</v>
       </c>
-      <c r="D4" s="66" t="s">
+      <c r="D4" s="71" t="s">
         <v>221</v>
       </c>
       <c r="E4" s="33" t="s">
@@ -7780,9 +9009,9 @@
       <c r="L4" s="6"/>
     </row>
     <row r="5" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B5" s="62"/>
-      <c r="C5" s="67"/>
-      <c r="D5" s="66"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="71"/>
       <c r="E5" s="33" t="s">
         <v>334</v>
       </c>
@@ -7801,9 +9030,9 @@
       <c r="L5" s="6"/>
     </row>
     <row r="6" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="62"/>
-      <c r="C6" s="67"/>
-      <c r="D6" s="66"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="70"/>
+      <c r="D6" s="71"/>
       <c r="E6" s="33" t="s">
         <v>334</v>
       </c>
@@ -7822,9 +9051,9 @@
       <c r="L6" s="6"/>
     </row>
     <row r="7" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B7" s="62"/>
-      <c r="C7" s="67"/>
-      <c r="D7" s="66"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="71"/>
       <c r="E7" s="33" t="s">
         <v>334</v>
       </c>
@@ -7843,9 +9072,9 @@
       <c r="L7" s="6"/>
     </row>
     <row r="8" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B8" s="62"/>
-      <c r="C8" s="67"/>
-      <c r="D8" s="66" t="s">
+      <c r="B8" s="61"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="71" t="s">
         <v>222</v>
       </c>
       <c r="E8" s="33" t="s">
@@ -7866,9 +9095,9 @@
       <c r="L8" s="6"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B9" s="62"/>
-      <c r="C9" s="67"/>
-      <c r="D9" s="66"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="71"/>
       <c r="E9" s="33" t="s">
         <v>334</v>
       </c>
@@ -7887,9 +9116,9 @@
       <c r="L9" s="6"/>
     </row>
     <row r="10" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="62"/>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="70" t="s">
         <v>225</v>
       </c>
       <c r="E10" s="34" t="s">
@@ -7910,9 +9139,9 @@
       <c r="L10" s="6"/>
     </row>
     <row r="11" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="62"/>
-      <c r="C11" s="67"/>
-      <c r="D11" s="67"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="70"/>
       <c r="E11" s="34" t="s">
         <v>333</v>
       </c>
@@ -7931,13 +9160,13 @@
       <c r="L11" s="6"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B12" s="62">
+      <c r="B12" s="61">
         <v>2</v>
       </c>
-      <c r="C12" s="67" t="s">
+      <c r="C12" s="70" t="s">
         <v>185</v>
       </c>
-      <c r="D12" s="66" t="s">
+      <c r="D12" s="71" t="s">
         <v>228</v>
       </c>
       <c r="E12" s="33" t="s">
@@ -7958,9 +9187,9 @@
       <c r="L12" s="6"/>
     </row>
     <row r="13" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B13" s="62"/>
-      <c r="C13" s="67"/>
-      <c r="D13" s="66"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="70"/>
+      <c r="D13" s="71"/>
       <c r="E13" s="33" t="s">
         <v>334</v>
       </c>
@@ -7979,9 +9208,9 @@
       <c r="L13" s="6"/>
     </row>
     <row r="14" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B14" s="62"/>
-      <c r="C14" s="67"/>
-      <c r="D14" s="66" t="s">
+      <c r="B14" s="61"/>
+      <c r="C14" s="70"/>
+      <c r="D14" s="71" t="s">
         <v>231</v>
       </c>
       <c r="E14" s="33" t="s">
@@ -8002,9 +9231,9 @@
       <c r="L14" s="6"/>
     </row>
     <row r="15" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B15" s="62"/>
-      <c r="C15" s="67"/>
-      <c r="D15" s="66"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="70"/>
+      <c r="D15" s="71"/>
       <c r="E15" s="33" t="s">
         <v>335</v>
       </c>
@@ -8023,13 +9252,13 @@
       <c r="L15" s="6"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B16" s="71">
+      <c r="B16" s="67">
         <v>3</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="70" t="s">
         <v>242</v>
       </c>
-      <c r="D16" s="66" t="s">
+      <c r="D16" s="71" t="s">
         <v>233</v>
       </c>
       <c r="E16" s="33" t="s">
@@ -8050,9 +9279,9 @@
       <c r="L16" s="6"/>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B17" s="72"/>
-      <c r="C17" s="67"/>
-      <c r="D17" s="66"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="70"/>
+      <c r="D17" s="71"/>
       <c r="E17" s="33" t="s">
         <v>336</v>
       </c>
@@ -8071,9 +9300,9 @@
       <c r="L17" s="6"/>
     </row>
     <row r="18" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B18" s="72"/>
-      <c r="C18" s="67"/>
-      <c r="D18" s="66"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="70"/>
+      <c r="D18" s="71"/>
       <c r="E18" s="33" t="s">
         <v>336</v>
       </c>
@@ -8092,9 +9321,9 @@
       <c r="L18" s="6"/>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B19" s="72"/>
-      <c r="C19" s="67"/>
-      <c r="D19" s="66" t="s">
+      <c r="B19" s="68"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="71" t="s">
         <v>243</v>
       </c>
       <c r="E19" s="33" t="s">
@@ -8115,9 +9344,9 @@
       <c r="L19" s="6"/>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B20" s="72"/>
-      <c r="C20" s="67"/>
-      <c r="D20" s="66"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="71"/>
       <c r="E20" s="33" t="s">
         <v>336</v>
       </c>
@@ -8136,9 +9365,9 @@
       <c r="L20" s="6"/>
     </row>
     <row r="21" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B21" s="72"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="66"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="71"/>
       <c r="E21" s="33" t="s">
         <v>336</v>
       </c>
@@ -8157,9 +9386,9 @@
       <c r="L21" s="6"/>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B22" s="73"/>
-      <c r="C22" s="67"/>
-      <c r="D22" s="66"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="71"/>
       <c r="E22" s="33" t="s">
         <v>336</v>
       </c>
@@ -8178,13 +9407,13 @@
       <c r="L22" s="6"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B23" s="62">
+      <c r="B23" s="61">
         <v>4</v>
       </c>
-      <c r="C23" s="67" t="s">
+      <c r="C23" s="70" t="s">
         <v>244</v>
       </c>
-      <c r="D23" s="66" t="s">
+      <c r="D23" s="71" t="s">
         <v>186</v>
       </c>
       <c r="E23" s="41">
@@ -8205,9 +9434,9 @@
       <c r="L23" s="6"/>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B24" s="62"/>
-      <c r="C24" s="67"/>
-      <c r="D24" s="66"/>
+      <c r="B24" s="61"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="71"/>
       <c r="E24" s="41">
         <v>44520</v>
       </c>
@@ -8226,9 +9455,9 @@
       <c r="L24" s="6"/>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B25" s="62"/>
-      <c r="C25" s="67"/>
-      <c r="D25" s="66"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="70"/>
+      <c r="D25" s="71"/>
       <c r="E25" s="41">
         <v>44520</v>
       </c>
@@ -8247,9 +9476,9 @@
       <c r="L25" s="6"/>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B26" s="62"/>
-      <c r="C26" s="67"/>
-      <c r="D26" s="66"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="70"/>
+      <c r="D26" s="71"/>
       <c r="E26" s="41">
         <v>44520</v>
       </c>
@@ -8268,9 +9497,9 @@
       <c r="L26" s="6"/>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B27" s="62"/>
-      <c r="C27" s="67"/>
-      <c r="D27" s="66"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="70"/>
+      <c r="D27" s="71"/>
       <c r="E27" s="41">
         <v>44520</v>
       </c>
@@ -8289,9 +9518,9 @@
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B28" s="62"/>
-      <c r="C28" s="67"/>
-      <c r="D28" s="66"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="70"/>
+      <c r="D28" s="71"/>
       <c r="E28" s="41">
         <v>44520</v>
       </c>
@@ -8310,9 +9539,9 @@
       <c r="L28" s="6"/>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B29" s="62"/>
-      <c r="C29" s="67"/>
-      <c r="D29" s="66"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="70"/>
+      <c r="D29" s="71"/>
       <c r="E29" s="41">
         <v>44520</v>
       </c>
@@ -8331,9 +9560,9 @@
       <c r="L29" s="6"/>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B30" s="62"/>
-      <c r="C30" s="67"/>
-      <c r="D30" s="66"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="70"/>
+      <c r="D30" s="71"/>
       <c r="E30" s="41">
         <v>44520</v>
       </c>
@@ -8352,9 +9581,9 @@
       <c r="L30" s="6"/>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B31" s="62"/>
-      <c r="C31" s="67"/>
-      <c r="D31" s="66"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="70"/>
+      <c r="D31" s="71"/>
       <c r="E31" s="41">
         <v>44520</v>
       </c>
@@ -8373,9 +9602,9 @@
       <c r="L31" s="6"/>
     </row>
     <row r="32" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B32" s="62"/>
-      <c r="C32" s="67"/>
-      <c r="D32" s="66"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="70"/>
+      <c r="D32" s="71"/>
       <c r="E32" s="41">
         <v>44520</v>
       </c>
@@ -8394,9 +9623,9 @@
       <c r="L32" s="6"/>
     </row>
     <row r="33" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B33" s="62"/>
-      <c r="C33" s="67"/>
-      <c r="D33" s="66"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="70"/>
+      <c r="D33" s="71"/>
       <c r="E33" s="41">
         <v>44520</v>
       </c>
@@ -8415,9 +9644,9 @@
       <c r="L33" s="6"/>
     </row>
     <row r="34" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B34" s="62"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="66"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="70"/>
+      <c r="D34" s="71"/>
       <c r="E34" s="41">
         <v>44520</v>
       </c>
@@ -8436,11 +9665,11 @@
       <c r="L34" s="6"/>
     </row>
     <row r="35" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B35" s="71">
+      <c r="B35" s="67">
         <v>5</v>
       </c>
-      <c r="C35" s="67"/>
-      <c r="D35" s="66" t="s">
+      <c r="C35" s="70"/>
+      <c r="D35" s="71" t="s">
         <v>187</v>
       </c>
       <c r="E35" s="41">
@@ -8461,9 +9690,9 @@
       <c r="L35" s="6"/>
     </row>
     <row r="36" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B36" s="72"/>
-      <c r="C36" s="67"/>
-      <c r="D36" s="66"/>
+      <c r="B36" s="68"/>
+      <c r="C36" s="70"/>
+      <c r="D36" s="71"/>
       <c r="E36" s="41">
         <v>44530</v>
       </c>
@@ -8482,9 +9711,9 @@
       <c r="L36" s="6"/>
     </row>
     <row r="37" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B37" s="72"/>
-      <c r="C37" s="67"/>
-      <c r="D37" s="66"/>
+      <c r="B37" s="68"/>
+      <c r="C37" s="70"/>
+      <c r="D37" s="71"/>
       <c r="E37" s="41">
         <v>44530</v>
       </c>
@@ -8503,9 +9732,9 @@
       <c r="L37" s="6"/>
     </row>
     <row r="38" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B38" s="72"/>
-      <c r="C38" s="67"/>
-      <c r="D38" s="66"/>
+      <c r="B38" s="68"/>
+      <c r="C38" s="70"/>
+      <c r="D38" s="71"/>
       <c r="E38" s="41">
         <v>44530</v>
       </c>
@@ -8524,9 +9753,9 @@
       <c r="L38" s="6"/>
     </row>
     <row r="39" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B39" s="72"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="66"/>
+      <c r="B39" s="68"/>
+      <c r="C39" s="70"/>
+      <c r="D39" s="71"/>
       <c r="E39" s="41">
         <v>44530</v>
       </c>
@@ -8545,9 +9774,9 @@
       <c r="L39" s="6"/>
     </row>
     <row r="40" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B40" s="73"/>
-      <c r="C40" s="67"/>
-      <c r="D40" s="66"/>
+      <c r="B40" s="69"/>
+      <c r="C40" s="70"/>
+      <c r="D40" s="71"/>
       <c r="E40" s="41">
         <v>44530</v>
       </c>
@@ -8566,10 +9795,10 @@
       <c r="L40" s="6"/>
     </row>
     <row r="41" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B41" s="62">
+      <c r="B41" s="61">
         <v>6</v>
       </c>
-      <c r="C41" s="68" t="s">
+      <c r="C41" s="72" t="s">
         <v>250</v>
       </c>
       <c r="D41" s="11" t="s">
@@ -8593,8 +9822,8 @@
       <c r="L41" s="6"/>
     </row>
     <row r="42" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B42" s="62"/>
-      <c r="C42" s="69"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="73"/>
       <c r="D42" s="6" t="s">
         <v>253</v>
       </c>
@@ -8616,8 +9845,8 @@
       <c r="L42" s="6"/>
     </row>
     <row r="43" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B43" s="62"/>
-      <c r="C43" s="70"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="74"/>
       <c r="D43" s="33" t="s">
         <v>254</v>
       </c>
@@ -8639,13 +9868,13 @@
       <c r="L43" s="6"/>
     </row>
     <row r="44" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B44" s="62">
+      <c r="B44" s="61">
         <v>7</v>
       </c>
-      <c r="C44" s="67" t="s">
+      <c r="C44" s="70" t="s">
         <v>244</v>
       </c>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="71" t="s">
         <v>189</v>
       </c>
       <c r="E44" s="41">
@@ -8666,9 +9895,9 @@
       <c r="L44" s="6"/>
     </row>
     <row r="45" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B45" s="62"/>
-      <c r="C45" s="67"/>
-      <c r="D45" s="66"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="70"/>
+      <c r="D45" s="71"/>
       <c r="E45" s="41">
         <v>44561</v>
       </c>
@@ -8687,9 +9916,9 @@
       <c r="L45" s="6"/>
     </row>
     <row r="46" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B46" s="62"/>
-      <c r="C46" s="67"/>
-      <c r="D46" s="66"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="70"/>
+      <c r="D46" s="71"/>
       <c r="E46" s="41">
         <v>44561</v>
       </c>
@@ -8708,9 +9937,9 @@
       <c r="L46" s="6"/>
     </row>
     <row r="47" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B47" s="62"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="66"/>
+      <c r="B47" s="61"/>
+      <c r="C47" s="70"/>
+      <c r="D47" s="71"/>
       <c r="E47" s="41">
         <v>44561</v>
       </c>
@@ -8729,9 +9958,9 @@
       <c r="L47" s="6"/>
     </row>
     <row r="48" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B48" s="62"/>
-      <c r="C48" s="67"/>
-      <c r="D48" s="66"/>
+      <c r="B48" s="61"/>
+      <c r="C48" s="70"/>
+      <c r="D48" s="71"/>
       <c r="E48" s="41">
         <v>44561</v>
       </c>
@@ -8750,9 +9979,9 @@
       <c r="L48" s="6"/>
     </row>
     <row r="49" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B49" s="62"/>
-      <c r="C49" s="67"/>
-      <c r="D49" s="66"/>
+      <c r="B49" s="61"/>
+      <c r="C49" s="70"/>
+      <c r="D49" s="71"/>
       <c r="E49" s="41">
         <v>44561</v>
       </c>
@@ -8771,9 +10000,9 @@
       <c r="L49" s="6"/>
     </row>
     <row r="50" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B50" s="62"/>
-      <c r="C50" s="67"/>
-      <c r="D50" s="66"/>
+      <c r="B50" s="61"/>
+      <c r="C50" s="70"/>
+      <c r="D50" s="71"/>
       <c r="E50" s="41">
         <v>44561</v>
       </c>
@@ -8792,10 +10021,10 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B51" s="62">
+      <c r="B51" s="61">
         <v>6</v>
       </c>
-      <c r="C51" s="67" t="s">
+      <c r="C51" s="70" t="s">
         <v>250</v>
       </c>
       <c r="D51" s="33" t="s">
@@ -8819,8 +10048,8 @@
       <c r="L51" s="6"/>
     </row>
     <row r="52" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B52" s="62"/>
-      <c r="C52" s="67"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="70"/>
       <c r="D52" s="33" t="s">
         <v>253</v>
       </c>
@@ -8842,8 +10071,8 @@
       <c r="L52" s="6"/>
     </row>
     <row r="53" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="62"/>
-      <c r="C53" s="67"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="70"/>
       <c r="D53" s="33" t="s">
         <v>254</v>
       </c>
@@ -8865,13 +10094,13 @@
       <c r="L53" s="6"/>
     </row>
     <row r="54" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B54" s="62">
+      <c r="B54" s="61">
         <v>7</v>
       </c>
-      <c r="C54" s="67" t="s">
+      <c r="C54" s="70" t="s">
         <v>256</v>
       </c>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="71" t="s">
         <v>193</v>
       </c>
       <c r="E54" s="41">
@@ -8892,9 +10121,9 @@
       <c r="L54" s="6"/>
     </row>
     <row r="55" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B55" s="62"/>
-      <c r="C55" s="67"/>
-      <c r="D55" s="66"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="70"/>
+      <c r="D55" s="71"/>
       <c r="E55" s="41">
         <v>44578</v>
       </c>
@@ -8913,9 +10142,9 @@
       <c r="L55" s="6"/>
     </row>
     <row r="56" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B56" s="62"/>
-      <c r="C56" s="67"/>
-      <c r="D56" s="66"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="71"/>
       <c r="E56" s="41">
         <v>44578</v>
       </c>
@@ -8934,9 +10163,9 @@
       <c r="L56" s="6"/>
     </row>
     <row r="57" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B57" s="62"/>
-      <c r="C57" s="67"/>
-      <c r="D57" s="66"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="71"/>
       <c r="E57" s="41">
         <v>44581</v>
       </c>
@@ -8955,13 +10184,13 @@
       <c r="L57" s="6"/>
     </row>
     <row r="58" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B58" s="62">
+      <c r="B58" s="61">
         <v>8</v>
       </c>
-      <c r="C58" s="67" t="s">
+      <c r="C58" s="70" t="s">
         <v>261</v>
       </c>
-      <c r="D58" s="66" t="s">
+      <c r="D58" s="71" t="s">
         <v>262</v>
       </c>
       <c r="E58" s="33" t="s">
@@ -8982,9 +10211,9 @@
       <c r="L58" s="6"/>
     </row>
     <row r="59" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B59" s="62"/>
-      <c r="C59" s="67"/>
-      <c r="D59" s="66"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="70"/>
+      <c r="D59" s="71"/>
       <c r="E59" s="33" t="s">
         <v>333</v>
       </c>
@@ -9003,9 +10232,9 @@
       <c r="L59" s="6"/>
     </row>
     <row r="60" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B60" s="62"/>
-      <c r="C60" s="67"/>
-      <c r="D60" s="66"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="71"/>
       <c r="E60" s="33" t="s">
         <v>333</v>
       </c>
@@ -9024,9 +10253,9 @@
       <c r="L60" s="6"/>
     </row>
     <row r="61" spans="2:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="B61" s="62"/>
-      <c r="C61" s="67"/>
-      <c r="D61" s="66" t="s">
+      <c r="B61" s="61"/>
+      <c r="C61" s="70"/>
+      <c r="D61" s="71" t="s">
         <v>266</v>
       </c>
       <c r="E61" s="41">
@@ -9047,9 +10276,9 @@
       <c r="L61" s="6"/>
     </row>
     <row r="62" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B62" s="62"/>
-      <c r="C62" s="67"/>
-      <c r="D62" s="66"/>
+      <c r="B62" s="61"/>
+      <c r="C62" s="70"/>
+      <c r="D62" s="71"/>
       <c r="E62" s="41">
         <v>44583</v>
       </c>
@@ -9068,10 +10297,10 @@
       <c r="L62" s="6"/>
     </row>
     <row r="63" spans="2:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="B63" s="62">
+      <c r="B63" s="61">
         <v>9</v>
       </c>
-      <c r="C63" s="67" t="s">
+      <c r="C63" s="70" t="s">
         <v>269</v>
       </c>
       <c r="D63" s="34" t="s">
@@ -9095,8 +10324,8 @@
       <c r="L63" s="6"/>
     </row>
     <row r="64" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B64" s="62"/>
-      <c r="C64" s="67"/>
+      <c r="B64" s="61"/>
+      <c r="C64" s="70"/>
       <c r="D64" s="6" t="s">
         <v>272</v>
       </c>
@@ -9119,6 +10348,34 @@
     </row>
   </sheetData>
   <mergeCells count="44">
+    <mergeCell ref="B23:B34"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B58:B62"/>
+    <mergeCell ref="B54:B57"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="B44:B50"/>
+    <mergeCell ref="B41:B43"/>
+    <mergeCell ref="D35:D40"/>
+    <mergeCell ref="D23:D34"/>
+    <mergeCell ref="C23:C40"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="D58:D60"/>
+    <mergeCell ref="C58:C62"/>
+    <mergeCell ref="D54:D57"/>
+    <mergeCell ref="C54:C57"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="D44:D50"/>
+    <mergeCell ref="C44:C50"/>
+    <mergeCell ref="C41:C43"/>
+    <mergeCell ref="B12:B15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="D12:D13"/>
+    <mergeCell ref="C12:C15"/>
+    <mergeCell ref="D19:D22"/>
+    <mergeCell ref="D16:D18"/>
+    <mergeCell ref="C16:C22"/>
+    <mergeCell ref="B16:B22"/>
     <mergeCell ref="K2:K3"/>
     <mergeCell ref="D2:D3"/>
     <mergeCell ref="L2:L3"/>
@@ -9135,34 +10392,6 @@
     <mergeCell ref="C4:C11"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="I2:I3"/>
-    <mergeCell ref="B12:B15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="D12:D13"/>
-    <mergeCell ref="C12:C15"/>
-    <mergeCell ref="D19:D22"/>
-    <mergeCell ref="D16:D18"/>
-    <mergeCell ref="C16:C22"/>
-    <mergeCell ref="B16:B22"/>
-    <mergeCell ref="D35:D40"/>
-    <mergeCell ref="D23:D34"/>
-    <mergeCell ref="C23:C40"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="D61:D62"/>
-    <mergeCell ref="D58:D60"/>
-    <mergeCell ref="C58:C62"/>
-    <mergeCell ref="D54:D57"/>
-    <mergeCell ref="C54:C57"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D44:D50"/>
-    <mergeCell ref="C44:C50"/>
-    <mergeCell ref="C41:C43"/>
-    <mergeCell ref="B23:B34"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="B58:B62"/>
-    <mergeCell ref="B54:B57"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="B44:B50"/>
-    <mergeCell ref="B41:B43"/>
   </mergeCells>
   <conditionalFormatting sqref="K2">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="equal">

</xml_diff>